<commit_message>
update import export, update timeline
</commit_message>
<xml_diff>
--- a/Dokumente/Timeline/Timeline.xlsx
+++ b/Dokumente/Timeline/Timeline.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1038" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1638" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="57">
   <si>
     <t>Arnstorfer Dominik</t>
   </si>
@@ -192,6 +192,15 @@
   </si>
   <si>
     <t xml:space="preserve">Neue Icons suchen </t>
+  </si>
+  <si>
+    <t>General Settings erstellen</t>
+  </si>
+  <si>
+    <t>Ordnerstruktur geupdated</t>
+  </si>
+  <si>
+    <t>Import / Export erstellen</t>
   </si>
 </sst>
 </file>
@@ -323,7 +332,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="6" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -331,16 +340,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -352,7 +359,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Besuchter Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -674,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:H103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="93" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I80" sqref="I80"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="93" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J100" sqref="J100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -712,81 +722,81 @@
       <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="5"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="5"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="7"/>
+      <c r="G4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="5"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5" t="s">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="5"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="3">
         <f>SUM(B2:B5)</f>
         <v>4</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="3"/>
@@ -804,81 +814,81 @@
       <c r="B8" s="3">
         <v>1</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5" t="s">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5" t="s">
+      <c r="F8" s="7"/>
+      <c r="G8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="5"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5" t="s">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5" t="s">
+      <c r="F9" s="7"/>
+      <c r="G9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="5"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5" t="s">
+      <c r="F10" s="7"/>
+      <c r="G10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="5"/>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="3">
         <v>1</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5" t="s">
+      <c r="F11" s="7"/>
+      <c r="G11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="5"/>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="3">
         <f>SUM(B8:B11)</f>
         <v>4</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="3"/>
@@ -896,81 +906,81 @@
       <c r="B14" s="3">
         <v>1</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5" t="s">
+      <c r="D14" s="7"/>
+      <c r="E14" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5" t="s">
+      <c r="F14" s="7"/>
+      <c r="G14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="5"/>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="3">
         <v>1</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5" t="s">
+      <c r="D15" s="7"/>
+      <c r="E15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5" t="s">
+      <c r="F15" s="7"/>
+      <c r="G15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="5"/>
+      <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="3">
         <v>1</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5" t="s">
+      <c r="D16" s="7"/>
+      <c r="E16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5" t="s">
+      <c r="F16" s="7"/>
+      <c r="G16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="5"/>
+      <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="3">
         <v>1</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5" t="s">
+      <c r="D17" s="7"/>
+      <c r="E17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5" t="s">
+      <c r="F17" s="7"/>
+      <c r="G17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="5"/>
+      <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="3">
         <f>SUM(B14:B17)</f>
         <v>4</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="3"/>
@@ -988,98 +998,98 @@
       <c r="B20" s="3">
         <v>0.5</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="8" t="s">
+      <c r="D20" s="7"/>
+      <c r="E20" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="5" t="s">
+      <c r="F20" s="12"/>
+      <c r="G20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="5"/>
+      <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="3">
         <v>1.5</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5" t="s">
+      <c r="D21" s="7"/>
+      <c r="E21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5" t="s">
+      <c r="F21" s="7"/>
+      <c r="G21" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H21" s="5"/>
+      <c r="H21" s="7"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="3">
         <v>0.5</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5" t="s">
+      <c r="D22" s="7"/>
+      <c r="E22" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5" t="s">
+      <c r="F22" s="7"/>
+      <c r="G22" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="5"/>
+      <c r="H22" s="7"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="3">
         <v>0.5</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5" t="s">
+      <c r="D23" s="7"/>
+      <c r="E23" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5" t="s">
+      <c r="F23" s="7"/>
+      <c r="G23" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H23" s="5"/>
+      <c r="H23" s="7"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="3">
         <v>1</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5" t="s">
+      <c r="D24" s="7"/>
+      <c r="E24" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5" t="s">
+      <c r="F24" s="7"/>
+      <c r="G24" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="5"/>
+      <c r="H24" s="7"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="3">
         <f>SUM(B20:B24)</f>
         <v>4</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2">
@@ -1088,90 +1098,90 @@
       <c r="B27" s="3">
         <v>1</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="8" t="s">
+      <c r="D27" s="7"/>
+      <c r="E27" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="5" t="s">
+      <c r="F27" s="12"/>
+      <c r="G27" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H27" s="5"/>
+      <c r="H27" s="7"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="3">
         <v>1</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5" t="s">
+      <c r="D28" s="7"/>
+      <c r="E28" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5" t="s">
+      <c r="F28" s="7"/>
+      <c r="G28" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H28" s="5"/>
+      <c r="H28" s="7"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="3">
         <v>1</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5" t="s">
+      <c r="D29" s="7"/>
+      <c r="E29" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5" t="s">
+      <c r="F29" s="7"/>
+      <c r="G29" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H29" s="5"/>
+      <c r="H29" s="7"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="3">
         <v>1</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5" t="s">
+      <c r="D30" s="7"/>
+      <c r="E30" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5" t="s">
+      <c r="F30" s="7"/>
+      <c r="G30" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H30" s="5"/>
+      <c r="H30" s="7"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="3">
         <f>SUM(B27:B30)</f>
         <v>4</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" s="3"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2">
@@ -1181,90 +1191,90 @@
       <c r="B33" s="3">
         <v>1</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="8" t="s">
+      <c r="D33" s="7"/>
+      <c r="E33" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F33" s="8"/>
-      <c r="G33" s="5" t="s">
+      <c r="F33" s="12"/>
+      <c r="G33" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H33" s="5"/>
+      <c r="H33" s="7"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" s="3">
         <v>1</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5" t="s">
+      <c r="D34" s="7"/>
+      <c r="E34" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5" t="s">
+      <c r="F34" s="7"/>
+      <c r="G34" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H34" s="5"/>
+      <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" s="3">
         <v>1</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5" t="s">
+      <c r="D35" s="7"/>
+      <c r="E35" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5" t="s">
+      <c r="F35" s="7"/>
+      <c r="G35" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H35" s="5"/>
+      <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" s="3">
         <v>1</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5" t="s">
+      <c r="D36" s="7"/>
+      <c r="E36" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5" t="s">
+      <c r="F36" s="7"/>
+      <c r="G36" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H36" s="5"/>
+      <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="3">
         <f>SUM(B33:B36)</f>
         <v>4</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" s="3"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2">
@@ -1278,10 +1288,10 @@
         <v>29</v>
       </c>
       <c r="D39" s="6"/>
-      <c r="E39" s="7" t="s">
+      <c r="E39" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F39" s="7"/>
+      <c r="F39" s="8"/>
       <c r="G39" s="6" t="s">
         <v>29</v>
       </c>
@@ -1295,10 +1305,10 @@
         <v>29</v>
       </c>
       <c r="D40" s="6"/>
-      <c r="E40" s="7" t="s">
+      <c r="E40" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F40" s="7"/>
+      <c r="F40" s="8"/>
       <c r="G40" s="6" t="s">
         <v>29</v>
       </c>
@@ -1312,10 +1322,10 @@
         <v>30</v>
       </c>
       <c r="D41" s="6"/>
-      <c r="E41" s="7" t="s">
+      <c r="E41" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F41" s="7"/>
+      <c r="F41" s="8"/>
       <c r="G41" s="6" t="s">
         <v>31</v>
       </c>
@@ -1329,10 +1339,10 @@
         <v>30</v>
       </c>
       <c r="D42" s="6"/>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F42" s="7"/>
+      <c r="F42" s="8"/>
       <c r="G42" s="6" t="s">
         <v>31</v>
       </c>
@@ -1343,12 +1353,12 @@
         <f>SUM(B39:B42)</f>
         <v>4</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2">
@@ -1427,12 +1437,12 @@
         <f>SUM(B45:B48)</f>
         <v>4</v>
       </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="2">
@@ -1446,10 +1456,10 @@
         <v>34</v>
       </c>
       <c r="D51" s="6"/>
-      <c r="E51" s="7" t="s">
+      <c r="E51" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F51" s="7"/>
+      <c r="F51" s="8"/>
       <c r="G51" s="6" t="s">
         <v>35</v>
       </c>
@@ -1463,10 +1473,10 @@
         <v>34</v>
       </c>
       <c r="D52" s="6"/>
-      <c r="E52" s="7" t="s">
+      <c r="E52" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F52" s="7"/>
+      <c r="F52" s="8"/>
       <c r="G52" s="6" t="s">
         <v>35</v>
       </c>
@@ -1497,10 +1507,10 @@
         <v>34</v>
       </c>
       <c r="D54" s="6"/>
-      <c r="E54" s="5" t="s">
+      <c r="E54" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F54" s="5"/>
+      <c r="F54" s="7"/>
       <c r="G54" s="6" t="s">
         <v>35</v>
       </c>
@@ -1511,12 +1521,12 @@
         <f>SUM(B51:B54)</f>
         <v>4</v>
       </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="2">
@@ -1595,12 +1605,12 @@
         <f>SUM(B57:B60)</f>
         <v>4</v>
       </c>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="2">
@@ -1614,10 +1624,10 @@
         <v>41</v>
       </c>
       <c r="D63" s="6"/>
-      <c r="E63" s="7" t="s">
+      <c r="E63" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F63" s="7"/>
+      <c r="F63" s="8"/>
       <c r="G63" s="6" t="s">
         <v>41</v>
       </c>
@@ -1648,10 +1658,10 @@
         <v>39</v>
       </c>
       <c r="D65" s="6"/>
-      <c r="E65" s="5" t="s">
+      <c r="E65" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F65" s="5"/>
+      <c r="F65" s="7"/>
       <c r="G65" s="6" t="s">
         <v>41</v>
       </c>
@@ -1661,30 +1671,30 @@
       <c r="B66" s="3">
         <v>1</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5" t="s">
+      <c r="D66" s="7"/>
+      <c r="E66" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5" t="s">
+      <c r="F66" s="7"/>
+      <c r="G66" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H66" s="5"/>
+      <c r="H66" s="7"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B67" s="3">
         <f>SUM(B63:B66)</f>
         <v>4</v>
       </c>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="2">
@@ -1698,7 +1708,7 @@
         <v>43</v>
       </c>
       <c r="D69" s="6"/>
-      <c r="H69" s="12" t="s">
+      <c r="H69" s="5" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1710,7 +1720,7 @@
         <v>43</v>
       </c>
       <c r="D70" s="6"/>
-      <c r="H70" s="12" t="s">
+      <c r="H70" s="5" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1722,7 +1732,7 @@
         <v>44</v>
       </c>
       <c r="D71" s="6"/>
-      <c r="H71" s="12" t="s">
+      <c r="H71" s="5" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1733,8 +1743,8 @@
       <c r="C72" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D72" s="5"/>
-      <c r="H72" s="12" t="s">
+      <c r="D72" s="7"/>
+      <c r="H72" s="5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1743,8 +1753,8 @@
         <f>SUM(B69:B72)</f>
         <v>4</v>
       </c>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="2">
@@ -1758,7 +1768,7 @@
         <v>46</v>
       </c>
       <c r="D75" s="6"/>
-      <c r="H75" s="12" t="s">
+      <c r="H75" s="5" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1770,7 +1780,7 @@
         <v>47</v>
       </c>
       <c r="D76" s="6"/>
-      <c r="H76" s="12" t="s">
+      <c r="H76" s="5" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1782,7 +1792,7 @@
         <v>48</v>
       </c>
       <c r="D77" s="6"/>
-      <c r="H77" s="12" t="s">
+      <c r="H77" s="5" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1794,7 +1804,7 @@
         <v>48</v>
       </c>
       <c r="D78" s="6"/>
-      <c r="H78" s="12" t="s">
+      <c r="H78" s="5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1803,13 +1813,11 @@
         <f>SUM(B75:B78)</f>
         <v>4</v>
       </c>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="H80" s="12" t="s">
-        <v>52</v>
-      </c>
+      <c r="H80" s="5"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="2">
@@ -1823,7 +1831,7 @@
         <v>48</v>
       </c>
       <c r="D81" s="6"/>
-      <c r="H81" s="12" t="s">
+      <c r="H81" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1835,7 +1843,7 @@
         <v>48</v>
       </c>
       <c r="D82" s="6"/>
-      <c r="H82" s="12" t="s">
+      <c r="H82" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1847,7 +1855,7 @@
         <v>48</v>
       </c>
       <c r="D83" s="6"/>
-      <c r="H83" s="12" t="s">
+      <c r="H83" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1859,101 +1867,227 @@
         <v>48</v>
       </c>
       <c r="D84" s="6"/>
+      <c r="H84" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B85" s="3">
         <f>SUM(B81:B84)</f>
         <v>4</v>
       </c>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" s="2">
+        <f>A81+7</f>
+        <v>43088</v>
+      </c>
+      <c r="B87" s="13">
+        <v>1</v>
+      </c>
+      <c r="H87" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B88" s="13">
+        <v>1</v>
+      </c>
+      <c r="H88" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B89" s="13">
+        <v>1</v>
+      </c>
+      <c r="H89" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B90" s="13">
+        <v>1</v>
+      </c>
+      <c r="H90" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B91" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" s="2">
+        <f>A87+21</f>
+        <v>43109</v>
+      </c>
+      <c r="B93" s="13">
+        <v>1</v>
+      </c>
+      <c r="H93" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B94" s="13">
+        <v>1</v>
+      </c>
+      <c r="H94" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B95" s="13">
+        <v>1</v>
+      </c>
+      <c r="H95" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B96" s="13">
+        <v>1</v>
+      </c>
+      <c r="H96" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B97" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" s="2">
+        <f>A93+7</f>
+        <v>43116</v>
+      </c>
+      <c r="B99" s="13">
+        <v>1</v>
+      </c>
+      <c r="H99" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B100" s="13">
+        <v>1</v>
+      </c>
+      <c r="H100" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B101" s="13">
+        <v>1</v>
+      </c>
+      <c r="H101" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B102" s="13">
+        <v>1</v>
+      </c>
+      <c r="H102" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B103" s="13">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="192">
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="G61:H61"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="G63:H63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="G64:H64"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="C9:D9"/>
@@ -1978,90 +2112,90 @@
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="G64:H64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="G67:H67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>